<commit_message>
feat: remove aditional index
</commit_message>
<xml_diff>
--- a/03_arquivos/07_planilhas/abas_planilhas.xlsx
+++ b/03_arquivos/07_planilhas/abas_planilhas.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,759 +436,654 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>Telefones</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Telefones</t>
+          <t>email</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>receita</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>David Westmark</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="B2" t="n">
         <v>90950816</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>davidw@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>553410.95</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Jose Prendergast</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>98884330</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>josep@gmail.com</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D3" t="n">
         <v>609898.3</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Dannie Hazard</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="B4" t="n">
         <v>95704128</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>dannieh@gmail.com</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="D4" t="n">
         <v>393376.53</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Isabella Mills</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="B5" t="n">
         <v>96001536</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>isabellam@gmail.com</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>265234.22</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Summer Godwin</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="B6" t="n">
         <v>96767892</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>summerg@gmail.com</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>357351.67</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Tiffany Caldwell</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="B7" t="n">
         <v>94693709</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>tiffanyc@gmail.com</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
         <v>429511.14</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Jon Ruud</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>93196046</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>jonr@gmail.com</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>721998.84</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>James Johnson</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="B9" t="n">
         <v>99667512</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>jamesj@gmail.com</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="D9" t="n">
         <v>371219.03</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Alexander Jones</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="B10" t="n">
         <v>99048721</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>alexanderj@gmail.com</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="D10" t="n">
         <v>906479.67</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Anthony Burrus</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="B11" t="n">
         <v>98034818</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>anthonyb@gmail.com</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>122323.72</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Louise Lampe</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="B12" t="n">
         <v>92738972</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>louisel@gmail.com</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>146207.73</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Stanley Peterson</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="B13" t="n">
         <v>92024858</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>stanleyp@gmail.com</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>305627.26</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Daisy Greis</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>96465571</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>daisyg@gmail.com</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>98646.87</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Brenda Joyce</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="B15" t="n">
         <v>91237474</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>brendaj@gmail.com</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="D15" t="n">
         <v>673071.48</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>James Delperdang</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="B16" t="n">
         <v>97806472</v>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>jamesd@gmail.com</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="D16" t="n">
         <v>367005.38</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Paul Harris</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="B17" t="n">
         <v>91697926</v>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>paulh@gmail.com</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="D17" t="n">
         <v>439501.66</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Kenneth Garcia</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="B18" t="n">
         <v>98280326</v>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>kennethg@gmail.com</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="D18" t="n">
         <v>632618.67</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Annie Luppino</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="B19" t="n">
         <v>97351397</v>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>anniel@gmail.com</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="D19" t="n">
         <v>627363.5600000001</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Douglas Moss</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="B20" t="n">
         <v>97472148</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>douglasm@gmail.com</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>561447.86</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Rodney Perkins</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="B21" t="n">
         <v>95784925</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>rodneyp@gmail.com</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>147385.51</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Andrew Alvarado</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="B22" t="n">
         <v>94105467</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>andrewa@gmail.com</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="D22" t="n">
         <v>830737.4300000001</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Lisa Green</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="B23" t="n">
         <v>99472405</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>lisag@gmail.com</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="D23" t="n">
         <v>100154.02</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Velma Teague</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="B24" t="n">
         <v>93931898</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>velmat@gmail.com</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="D24" t="n">
         <v>653379.42</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Loretta Valencia</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="B25" t="n">
         <v>99469512</v>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>lorettav@gmail.com</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="D25" t="n">
         <v>849025.23</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Sandra Lank</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="B26" t="n">
         <v>91820996</v>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>sandral@gmail.com</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="D26" t="n">
         <v>396636.38</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Charles Grimaldo</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="B27" t="n">
         <v>98547715</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>charlesg@gmail.com</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="D27" t="n">
         <v>889349.88</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Troy Makris</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="B28" t="n">
         <v>96648633</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>troym@gmail.com</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="D28" t="n">
         <v>620966.4300000001</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Robert Wortham</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="B29" t="n">
         <v>99848030</v>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>robertw@gmail.com</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="D29" t="n">
         <v>452916.55</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Pablo Jones</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="B30" t="n">
         <v>92600402</v>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>pabloj@gmail.com</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="D30" t="n">
         <v>647857.11</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Theresa Battle</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="B31" t="n">
         <v>90810826</v>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>theresab@gmail.com</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="D31" t="n">
         <v>318288.93</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Sara Savage</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="B32" t="n">
         <v>98178282</v>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>saras@gmail.com</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="D32" t="n">
         <v>581899.08</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Duane Piche</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="B33" t="n">
         <v>91019921</v>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>duanep@gmail.com</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="D33" t="n">
         <v>846228.08</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Janet Smith</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="B34" t="n">
         <v>96181888</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>janets@gmail.com</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="D34" t="n">
         <v>247271.65</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Tabitha Salamone</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="B35" t="n">
         <v>99927802</v>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>tabithas@gmail.com</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="D35" t="n">
         <v>107710.17</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Corey Park</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="B36" t="n">
         <v>93172449</v>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>coreyp@gmail.com</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="D36" t="n">
         <v>297007.91</v>
       </c>
     </row>
@@ -1203,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1212,1326 +1107,1140 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>Telefones</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Telefones</t>
+          <t>email</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>receita</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Perry Coley</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="B2" t="n">
         <v>99096127</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>perryc@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>693438.83</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Joseph Harris</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>95134411</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>josephh@gmail.com</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D3" t="n">
         <v>356460.71</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Heather Meurer</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="B4" t="n">
         <v>92003842</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>heatherm@gmail.com</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="D4" t="n">
         <v>411931.57</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Stanley Harvey</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="B5" t="n">
         <v>97958279</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>stanleyh@gmail.com</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>627605.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Noel Pratt</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="B6" t="n">
         <v>96327340</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>noelp@gmail.com</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>136521.52</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Carol Johnson</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="B7" t="n">
         <v>91189860</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>carolj@gmail.com</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
         <v>721311.15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Gloria Adair</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>96590170</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>gloriaa@gmail.com</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>574719.8199999999</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Lucina Dillard</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="B9" t="n">
         <v>99852825</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>lucinad@gmail.com</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="D9" t="n">
         <v>722455.4399999999</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Allen Cody</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="B10" t="n">
         <v>92343755</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>allenc@gmail.com</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="D10" t="n">
         <v>540641.4399999999</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Alexis Rivera</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="B11" t="n">
         <v>92213457</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>alexisr@gmail.com</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>15627.42</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Gary Rowell</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="B12" t="n">
         <v>97308042</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>garyr@gmail.com</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>962206.16</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>John Petty</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="B13" t="n">
         <v>95318023</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>johnp@gmail.com</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>1031006.7</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Charles Wilburn</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>99054376</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>charlesw@gmail.com</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>106729.28</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Jessie Chiles</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="B15" t="n">
         <v>90598962</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>jessiec@gmail.com</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="D15" t="n">
         <v>114492.96</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Leonard Appleby</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="B16" t="n">
         <v>94433903</v>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>leonarda@gmail.com</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="D16" t="n">
         <v>274662.38</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>David Thomas</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="B17" t="n">
         <v>95111618</v>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>davidt@gmail.com</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="D17" t="n">
         <v>501762.62</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Alexander Simms</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="B18" t="n">
         <v>97264971</v>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>alexanders@gmail.com</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="D18" t="n">
         <v>946767.55</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Nicole Murphy</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="B19" t="n">
         <v>93884865</v>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>nicolem@gmail.com</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="D19" t="n">
         <v>553661.99</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Amber Wells</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="B20" t="n">
         <v>91884498</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>amberw@gmail.com</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>308500.34</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Helen Gross</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="B21" t="n">
         <v>99881440</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>heleng@gmail.com</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>895850.63</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Glen Haworth</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="B22" t="n">
         <v>91793646</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>glenh@gmail.com</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="D22" t="n">
         <v>739481.8199999999</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>James Elliott</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="B23" t="n">
         <v>90686574</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>jamese@gmail.com</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="D23" t="n">
         <v>553655.09</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Stephanie Cheney</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="B24" t="n">
         <v>99411210</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>stephaniec@gmail.com</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="D24" t="n">
         <v>436716.21</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Oscar Ollie</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="B25" t="n">
         <v>90689608</v>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>oscaro@gmail.com</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="D25" t="n">
         <v>463195.1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Herbert Reed</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="B26" t="n">
         <v>98646551</v>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>herbertr@gmail.com</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="D26" t="n">
         <v>697767.45</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Walter Grey</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="B27" t="n">
         <v>91826722</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>walterg@gmail.com</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="D27" t="n">
         <v>841094.76</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Calvin Caughey</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="B28" t="n">
         <v>94875414</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>calvinc@gmail.com</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="D28" t="n">
         <v>384070.16</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Christina Rivera</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="B29" t="n">
         <v>95166964</v>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>christinar@gmail.com</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="D29" t="n">
         <v>838309.84</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Virginia Hernandez</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="B30" t="n">
         <v>90804876</v>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>virginiah@gmail.com</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="D30" t="n">
         <v>435987.24</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Tasha Johnson</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="B31" t="n">
         <v>98321899</v>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>tashaj@gmail.com</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="D31" t="n">
         <v>763784.5699999999</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Joyce Garcia</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="B32" t="n">
         <v>93983004</v>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>joyceg@gmail.com</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="D32" t="n">
         <v>759719.92</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>James Rios</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="B33" t="n">
         <v>98312946</v>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>jamesr@gmail.com</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="D33" t="n">
         <v>216204.27</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Michael Manning</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="B34" t="n">
         <v>92695409</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>michaelm@gmail.com</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="D34" t="n">
         <v>760778.28</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Robert Tyree</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="B35" t="n">
         <v>93698956</v>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>robertt@gmail.com</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="D35" t="n">
         <v>565550.86</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Maryann Davis</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="B36" t="n">
         <v>90347539</v>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>maryannd@gmail.com</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="D36" t="n">
         <v>1030011.79</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Kenneth Daniels</t>
         </is>
       </c>
-      <c r="C37" t="n">
+      <c r="B37" t="n">
         <v>95131452</v>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>kennethd@gmail.com</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="D37" t="n">
         <v>1038060.42</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Joann Coy</t>
         </is>
       </c>
-      <c r="C38" t="n">
+      <c r="B38" t="n">
         <v>97893800</v>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>joannc@gmail.com</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="D38" t="n">
         <v>467200.36</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
+      <c r="A39" t="inlineStr">
         <is>
           <t>Willie Simpson</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="B39" t="n">
         <v>90125156</v>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>willies@gmail.com</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="D39" t="n">
         <v>594964.9300000001</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Ralph Mihalik</t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="B40" t="n">
         <v>92502387</v>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>ralphm@gmail.com</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="D40" t="n">
         <v>754953.77</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
+      <c r="A41" t="inlineStr">
         <is>
           <t>John Beaudreault</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="B41" t="n">
         <v>92195423</v>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>johnb@gmail.com</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="D41" t="n">
         <v>332135.45</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
+      <c r="A42" t="inlineStr">
         <is>
           <t>Carlos Campbell</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="B42" t="n">
         <v>95937753</v>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>carlosc@gmail.com</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="D42" t="n">
         <v>490082.48</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
+      <c r="A43" t="inlineStr">
         <is>
           <t>Carole Ramsey</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="B43" t="n">
         <v>90324173</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>caroler@gmail.com</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="D43" t="n">
         <v>640266.2</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
+      <c r="A44" t="inlineStr">
         <is>
           <t>Olga Big</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="B44" t="n">
         <v>91413335</v>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>olgab@gmail.com</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="D44" t="n">
         <v>724350.6800000001</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
+      <c r="A45" t="inlineStr">
         <is>
           <t>James Eichmann</t>
         </is>
       </c>
-      <c r="C45" t="n">
+      <c r="B45" t="n">
         <v>90153690</v>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>jamese@gmail.com</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="D45" t="n">
         <v>401680.45</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
+      <c r="A46" t="inlineStr">
         <is>
           <t>Gwendolyn Johnson</t>
         </is>
       </c>
-      <c r="C46" t="n">
+      <c r="B46" t="n">
         <v>99938812</v>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>gwendolynj@gmail.com</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="D46" t="n">
         <v>951415.47</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
+      <c r="A47" t="inlineStr">
         <is>
           <t>James Garrison</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="B47" t="n">
         <v>95950404</v>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>jamesg@gmail.com</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="D47" t="n">
         <v>527462.02</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
+      <c r="A48" t="inlineStr">
         <is>
           <t>Deborah Edwards</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="B48" t="n">
         <v>98551287</v>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>deborahe@gmail.com</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="D48" t="n">
         <v>811703.6899999999</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
+      <c r="A49" t="inlineStr">
         <is>
           <t>Amy Carter</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="B49" t="n">
         <v>96641702</v>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>amyc@gmail.com</t>
         </is>
       </c>
-      <c r="E49" t="n">
+      <c r="D49" t="n">
         <v>949884.67</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
+      <c r="A50" t="inlineStr">
         <is>
           <t>Joshua Morris</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="B50" t="n">
         <v>94680786</v>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>joshuam@gmail.com</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="D50" t="n">
         <v>881121.61</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
+      <c r="A51" t="inlineStr">
         <is>
           <t>George Enright</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="B51" t="n">
         <v>91255718</v>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>georgee@gmail.com</t>
         </is>
       </c>
-      <c r="E51" t="n">
+      <c r="D51" t="n">
         <v>694509.92</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
+      <c r="A52" t="inlineStr">
         <is>
           <t>Gregory Manion</t>
         </is>
       </c>
-      <c r="C52" t="n">
+      <c r="B52" t="n">
         <v>91532841</v>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>gregorym@gmail.com</t>
         </is>
       </c>
-      <c r="E52" t="n">
+      <c r="D52" t="n">
         <v>873973.09</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
+      <c r="A53" t="inlineStr">
         <is>
           <t>Abby Ruivo</t>
         </is>
       </c>
-      <c r="C53" t="n">
+      <c r="B53" t="n">
         <v>96431018</v>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>abbyr@gmail.com</t>
         </is>
       </c>
-      <c r="E53" t="n">
+      <c r="D53" t="n">
         <v>51483.8</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
+      <c r="A54" t="inlineStr">
         <is>
           <t>Miriam Quintero</t>
         </is>
       </c>
-      <c r="C54" t="n">
+      <c r="B54" t="n">
         <v>99620307</v>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>miriamq@gmail.com</t>
         </is>
       </c>
-      <c r="E54" t="n">
+      <c r="D54" t="n">
         <v>558965.9300000001</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
+      <c r="A55" t="inlineStr">
         <is>
           <t>Samuel Menke</t>
         </is>
       </c>
-      <c r="C55" t="n">
+      <c r="B55" t="n">
         <v>96138561</v>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>samuelm@gmail.com</t>
         </is>
       </c>
-      <c r="E55" t="n">
+      <c r="D55" t="n">
         <v>59075.15</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
+      <c r="A56" t="inlineStr">
         <is>
           <t>Christopher Selmer</t>
         </is>
       </c>
-      <c r="C56" t="n">
+      <c r="B56" t="n">
         <v>93085102</v>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>christophers@gmail.com</t>
         </is>
       </c>
-      <c r="E56" t="n">
+      <c r="D56" t="n">
         <v>441909.35</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
+      <c r="A57" t="inlineStr">
         <is>
           <t>Minnie Miller</t>
         </is>
       </c>
-      <c r="C57" t="n">
+      <c r="B57" t="n">
         <v>95951629</v>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>minniem@gmail.com</t>
         </is>
       </c>
-      <c r="E57" t="n">
+      <c r="D57" t="n">
         <v>979834</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
+      <c r="A58" t="inlineStr">
         <is>
           <t>Penny Hawks</t>
         </is>
       </c>
-      <c r="C58" t="n">
+      <c r="B58" t="n">
         <v>92480197</v>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>pennyh@gmail.com</t>
         </is>
       </c>
-      <c r="E58" t="n">
+      <c r="D58" t="n">
         <v>865457.87</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
+      <c r="A59" t="inlineStr">
         <is>
           <t>Thomas Roszel</t>
         </is>
       </c>
-      <c r="C59" t="n">
+      <c r="B59" t="n">
         <v>96912286</v>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>thomasr@gmail.com</t>
         </is>
       </c>
-      <c r="E59" t="n">
+      <c r="D59" t="n">
         <v>788675.4</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
+      <c r="A60" t="inlineStr">
         <is>
           <t>Alexander Weyer</t>
         </is>
       </c>
-      <c r="C60" t="n">
+      <c r="B60" t="n">
         <v>92613321</v>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>alexanderw@gmail.com</t>
         </is>
       </c>
-      <c r="E60" t="n">
+      <c r="D60" t="n">
         <v>116204.77</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
+      <c r="A61" t="inlineStr">
         <is>
           <t>Nicole Kruchten</t>
         </is>
       </c>
-      <c r="C61" t="n">
+      <c r="B61" t="n">
         <v>93364830</v>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>nicolek@gmail.com</t>
         </is>
       </c>
-      <c r="E61" t="n">
+      <c r="D61" t="n">
         <v>580090.5699999999</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
+      <c r="A62" t="inlineStr">
         <is>
           <t>Marlene Bailey</t>
         </is>
       </c>
-      <c r="C62" t="n">
+      <c r="B62" t="n">
         <v>92362772</v>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>marleneb@gmail.com</t>
         </is>
       </c>
-      <c r="E62" t="n">
+      <c r="D62" t="n">
         <v>554748.34</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr">
+      <c r="A63" t="inlineStr">
         <is>
           <t>John Hippler</t>
         </is>
       </c>
-      <c r="C63" t="n">
+      <c r="B63" t="n">
         <v>90693278</v>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>johnh@gmail.com</t>
         </is>
       </c>
-      <c r="E63" t="n">
+      <c r="D63" t="n">
         <v>203865.87</v>
       </c>
     </row>
@@ -2546,7 +2255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2555,1074 +2264,924 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>Telefones</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Telefones</t>
+          <t>email</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>receita</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Patricia Tattershall</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="B2" t="n">
         <v>98044446</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>patriciat@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>668574.0600000001</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Heather Glaze</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>95077237</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>heatherg@gmail.com</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D3" t="n">
         <v>1004265.7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Eleanor Bryant</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="B4" t="n">
         <v>91781720</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>eleanorb@gmail.com</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="D4" t="n">
         <v>455441.52</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Luis Rivers</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="B5" t="n">
         <v>97699482</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>luisr@gmail.com</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>489375.3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Vicki Gonzalez</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="B6" t="n">
         <v>91817390</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>vickig@gmail.com</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>325227.19</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Jennifer Agro</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="B7" t="n">
         <v>96153764</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>jennifera@gmail.com</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="D7" t="n">
         <v>757243.71</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Andrew Nichols</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>97795098</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>andrewn@gmail.com</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>717447.88</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Leo Mendoza</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="B9" t="n">
         <v>90380924</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>leom@gmail.com</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="D9" t="n">
         <v>384309.22</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Mark Carroll</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="B10" t="n">
         <v>91910458</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>markc@gmail.com</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="D10" t="n">
         <v>357310.31</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Elisabeth Harper</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="B11" t="n">
         <v>92905786</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>elisabethh@gmail.com</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="D11" t="n">
         <v>493462.59</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Douglas Hope</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="B12" t="n">
         <v>90667755</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>douglash@gmail.com</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>659224.9300000001</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Donald Mcdonald</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="B13" t="n">
         <v>92951965</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>donaldm@gmail.com</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>519840.41</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Corey Odonell</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>98266809</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>coreyo@gmail.com</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>126171.98</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Wilson Johnson</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="B15" t="n">
         <v>96809589</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>wilsonj@gmail.com</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="D15" t="n">
         <v>552312.4</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Victoria Netolicky</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="B16" t="n">
         <v>94309739</v>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>victorian@gmail.com</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="D16" t="n">
         <v>386493.99</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Sandra Adams</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="B17" t="n">
         <v>93569460</v>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>sandraa@gmail.com</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="D17" t="n">
         <v>200217.51</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Audrey Gann</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="B18" t="n">
         <v>96707062</v>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>audreyg@gmail.com</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="D18" t="n">
         <v>423382.01</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Brittany Jackson</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="B19" t="n">
         <v>92282529</v>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>brittanyj@gmail.com</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="D19" t="n">
         <v>323928.98</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Thomas Stark</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="B20" t="n">
         <v>98889439</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>thomass@gmail.com</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>62429.12</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Brad Sprague</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="B21" t="n">
         <v>96826054</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>brads@gmail.com</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>950869.23</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Robin Swenson</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="B22" t="n">
         <v>98586973</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>robins@gmail.com</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="D22" t="n">
         <v>175538.94</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Richard Teeters</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="B23" t="n">
         <v>94504380</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>richardt@gmail.com</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="D23" t="n">
         <v>419019.9</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Bessie Ashford</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="B24" t="n">
         <v>99801896</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>bessiea@gmail.com</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="D24" t="n">
         <v>39580.01</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Jerry Roehl</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="B25" t="n">
         <v>93741991</v>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>jerryr@gmail.com</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="D25" t="n">
         <v>278987.8</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Marian Tyree</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="B26" t="n">
         <v>93402110</v>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>mariant@gmail.com</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="D26" t="n">
         <v>802467.4399999999</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Rod Mcgray</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="B27" t="n">
         <v>90958525</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>rodm@gmail.com</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="D27" t="n">
         <v>453456.45</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Jose Ramirez</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="B28" t="n">
         <v>91855010</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>joser@gmail.com</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="D28" t="n">
         <v>965087.6800000001</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Francene Lasiter</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="B29" t="n">
         <v>93720900</v>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>francenel@gmail.com</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="D29" t="n">
         <v>526915.03</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Matthew Sumrall</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="B30" t="n">
         <v>91797318</v>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>matthews@gmail.com</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="D30" t="n">
         <v>634677.77</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Jo Sheehan</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="B31" t="n">
         <v>95412213</v>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>jos@gmail.com</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="D31" t="n">
         <v>527533.96</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Marjorie Money</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="B32" t="n">
         <v>90128001</v>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>marjoriem@gmail.com</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="D32" t="n">
         <v>982111.51</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Marilyn Washington</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="B33" t="n">
         <v>97906603</v>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>marilynw@gmail.com</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="D33" t="n">
         <v>363463.91</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Clifton King</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="B34" t="n">
         <v>95059121</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>cliftonk@gmail.com</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="D34" t="n">
         <v>192447.75</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Sandra Soto</t>
         </is>
       </c>
-      <c r="C35" t="n">
+      <c r="B35" t="n">
         <v>95084768</v>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>sandras@gmail.com</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="D35" t="n">
         <v>1036275.78</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Beatrice Laporte</t>
         </is>
       </c>
-      <c r="C36" t="n">
+      <c r="B36" t="n">
         <v>96360010</v>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>beatricel@gmail.com</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="D36" t="n">
         <v>373860.01</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Mark Phipps</t>
         </is>
       </c>
-      <c r="C37" t="n">
+      <c r="B37" t="n">
         <v>91075457</v>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>markp@gmail.com</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="D37" t="n">
         <v>699729.66</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Colleen Russell</t>
         </is>
       </c>
-      <c r="C38" t="n">
+      <c r="B38" t="n">
         <v>91325538</v>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>colleenr@gmail.com</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="D38" t="n">
         <v>150917.36</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
+      <c r="A39" t="inlineStr">
         <is>
           <t>Susan Speed</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="B39" t="n">
         <v>96217165</v>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>susans@gmail.com</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="D39" t="n">
         <v>454321.09</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Gerardo Jackson</t>
         </is>
       </c>
-      <c r="C40" t="n">
+      <c r="B40" t="n">
         <v>98408497</v>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>gerardoj@gmail.com</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="D40" t="n">
         <v>840441.55</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
+      <c r="A41" t="inlineStr">
         <is>
           <t>Micheal Harder</t>
         </is>
       </c>
-      <c r="C41" t="n">
+      <c r="B41" t="n">
         <v>98334372</v>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>michealh@gmail.com</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="D41" t="n">
         <v>772321.28</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
+      <c r="A42" t="inlineStr">
         <is>
           <t>Diane Spence</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="B42" t="n">
         <v>93589154</v>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>dianes@gmail.com</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="D42" t="n">
         <v>319609.69</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
+      <c r="A43" t="inlineStr">
         <is>
           <t>Edward Stewart</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="B43" t="n">
         <v>96442312</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>edwards@gmail.com</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="D43" t="n">
         <v>860359.26</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
+      <c r="A44" t="inlineStr">
         <is>
           <t>Cathy Moreno</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="B44" t="n">
         <v>93348609</v>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>cathym@gmail.com</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="D44" t="n">
         <v>19199.16</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
+      <c r="A45" t="inlineStr">
         <is>
           <t>Manuel Kooser</t>
         </is>
       </c>
-      <c r="C45" t="n">
+      <c r="B45" t="n">
         <v>98067234</v>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>manuelk@gmail.com</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="D45" t="n">
         <v>972102.4300000001</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
+      <c r="A46" t="inlineStr">
         <is>
           <t>Laura Sanchez</t>
         </is>
       </c>
-      <c r="C46" t="n">
+      <c r="B46" t="n">
         <v>93067867</v>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>lauras@gmail.com</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="D46" t="n">
         <v>976367.54</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
+      <c r="A47" t="inlineStr">
         <is>
           <t>Donna Bender</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="B47" t="n">
         <v>93922256</v>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>donnab@gmail.com</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="D47" t="n">
         <v>975202.0699999999</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
+      <c r="A48" t="inlineStr">
         <is>
           <t>Lisa Hackett</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="B48" t="n">
         <v>98932937</v>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>lisah@gmail.com</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="D48" t="n">
         <v>121676.47</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
+      <c r="A49" t="inlineStr">
         <is>
           <t>Cynthia Balson</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="B49" t="n">
         <v>94181420</v>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>cynthiab@gmail.com</t>
         </is>
       </c>
-      <c r="E49" t="n">
+      <c r="D49" t="n">
         <v>687284.33</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
+      <c r="A50" t="inlineStr">
         <is>
           <t>Bradley Peterson</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="B50" t="n">
         <v>97747510</v>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>bradleyp@gmail.com</t>
         </is>
       </c>
-      <c r="E50" t="n">
+      <c r="D50" t="n">
         <v>110326.52</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
+      <c r="A51" t="inlineStr">
         <is>
           <t>Sylvester Newton</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="B51" t="n">
         <v>97310089</v>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>sylvestern@gmail.com</t>
         </is>
       </c>
-      <c r="E51" t="n">
+      <c r="D51" t="n">
         <v>276114.2</v>
       </c>
     </row>

</xml_diff>